<commit_message>
Add Mapbox y recorrido sur
</commit_message>
<xml_diff>
--- a/argentinaton/public/datasetEntregas.xlsx
+++ b/argentinaton/public/datasetEntregas.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="151">
   <si>
     <t>Rocamora 1012, Concepción del Uruguay Entre Ríos, Argentina</t>
   </si>
@@ -396,13 +396,94 @@
   </si>
   <si>
     <t>Rosario, argentina</t>
+  </si>
+  <si>
+    <t>Pehuajó, buenos aires</t>
+  </si>
+  <si>
+    <t>Villa Regina, Rio negro</t>
+  </si>
+  <si>
+    <t>Neuquén, Neuquen</t>
+  </si>
+  <si>
+    <t>Neuquén, Neuquen, Argentina</t>
+  </si>
+  <si>
+    <t>Picún Leufú, Neuquen, Argentina</t>
+  </si>
+  <si>
+    <t>San Martin de los Andes, Neuquen, Argentina</t>
+  </si>
+  <si>
+    <t>Villa La Angostura, neuquen, argentina</t>
+  </si>
+  <si>
+    <t>Bariloche, Rio Negro</t>
+  </si>
+  <si>
+    <t>Esquel, Chubut</t>
+  </si>
+  <si>
+    <t>Gobernador Costa, Chubut</t>
+  </si>
+  <si>
+    <t>Los Antiguos, Santa Cruz</t>
+  </si>
+  <si>
+    <t>Las Horquetas, Santa Cruz</t>
+  </si>
+  <si>
+    <t>El Chalten, Santa Cruz</t>
+  </si>
+  <si>
+    <t>El Calafate, Santa Cruz</t>
+  </si>
+  <si>
+    <t>Rio Gallegos, Santa Cruz</t>
+  </si>
+  <si>
+    <t>Rio Grande, Tierra del Fuego</t>
+  </si>
+  <si>
+    <t>Ushuaia, Tierra del Fuego</t>
+  </si>
+  <si>
+    <t>Puerto Santa Cruz, Santa Cruz</t>
+  </si>
+  <si>
+    <t>Las Heras, Santa Cruz</t>
+  </si>
+  <si>
+    <t>Comodoro Rivadavia, Chubut</t>
+  </si>
+  <si>
+    <t>Trelew, Chubut</t>
+  </si>
+  <si>
+    <t>Puerto Madryn, Chubut</t>
+  </si>
+  <si>
+    <t>Puerto Piramides, Chubut</t>
+  </si>
+  <si>
+    <t>Las Grutas, Rio Negro</t>
+  </si>
+  <si>
+    <t>Bahía Blanca, Buenos Aires</t>
+  </si>
+  <si>
+    <t>Azul, Buenos Aires</t>
+  </si>
+  <si>
+    <t>general acha, la pampa</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -410,31 +491,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00FFFF"/>
-        <bgColor rgb="FF00FFFF"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -442,32 +508,13 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -757,10 +804,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H48"/>
+  <dimension ref="A1:H83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="C48" sqref="C48"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="E83" sqref="E83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -768,7 +815,7 @@
     <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="99.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="49" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -785,7 +832,7 @@
       <c r="D1" t="s">
         <v>43</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>33</v>
       </c>
       <c r="F1" t="s">
@@ -802,7 +849,7 @@
       <c r="C2" t="s">
         <v>36</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2" s="1">
         <v>43292</v>
       </c>
       <c r="F2" t="s">
@@ -813,7 +860,7 @@
       <c r="C3" t="s">
         <v>114</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="1">
         <v>43298</v>
       </c>
       <c r="F3" t="s">
@@ -830,7 +877,7 @@
       <c r="C4" t="s">
         <v>123</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="1">
         <v>43299</v>
       </c>
       <c r="F4" t="s">
@@ -850,7 +897,7 @@
       <c r="C5" t="s">
         <v>118</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="1">
         <v>43300</v>
       </c>
       <c r="F5" t="s">
@@ -870,11 +917,10 @@
       <c r="B6" t="s">
         <v>98</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" t="s">
         <v>101</v>
       </c>
-      <c r="D6" s="1"/>
-      <c r="E6" s="3">
+      <c r="E6" s="1">
         <v>43300</v>
       </c>
       <c r="F6" t="s">
@@ -894,11 +940,10 @@
       <c r="B7" t="s">
         <v>97</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" t="s">
         <v>105</v>
       </c>
-      <c r="D7" s="5"/>
-      <c r="E7" s="2">
+      <c r="E7" s="1">
         <v>43301</v>
       </c>
       <c r="F7" t="s">
@@ -918,11 +963,10 @@
       <c r="B8" t="s">
         <v>97</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" t="s">
         <v>104</v>
       </c>
-      <c r="D8" s="5"/>
-      <c r="E8" s="2">
+      <c r="E8" s="1">
         <v>43301</v>
       </c>
       <c r="F8" t="s">
@@ -942,11 +986,10 @@
       <c r="B9" t="s">
         <v>96</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" t="s">
         <v>31</v>
       </c>
-      <c r="D9" s="5"/>
-      <c r="E9" s="2">
+      <c r="E9" s="1">
         <v>43302</v>
       </c>
       <c r="F9" t="s">
@@ -957,11 +1000,10 @@
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C10" s="1" t="s">
+      <c r="C10" t="s">
         <v>29</v>
       </c>
-      <c r="D10" s="1"/>
-      <c r="E10" s="4">
+      <c r="E10" s="1">
         <v>43303</v>
       </c>
       <c r="F10" t="s">
@@ -972,11 +1014,10 @@
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C11" s="1" t="s">
+      <c r="C11" t="s">
         <v>30</v>
       </c>
-      <c r="D11" s="1"/>
-      <c r="E11" s="2">
+      <c r="E11" s="1">
         <v>43303</v>
       </c>
       <c r="F11" t="s">
@@ -990,13 +1031,13 @@
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C12" s="1" t="s">
+      <c r="C12" t="s">
         <v>27</v>
       </c>
-      <c r="D12" s="1">
+      <c r="D12">
         <v>2</v>
       </c>
-      <c r="E12" s="2">
+      <c r="E12" s="1">
         <v>43304</v>
       </c>
       <c r="F12" t="s">
@@ -1007,11 +1048,10 @@
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C13" s="1" t="s">
+      <c r="C13" t="s">
         <v>28</v>
       </c>
-      <c r="D13" s="1"/>
-      <c r="E13" s="2">
+      <c r="E13" s="1">
         <v>43304</v>
       </c>
       <c r="F13" t="s">
@@ -1022,11 +1062,10 @@
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C14" s="1" t="s">
+      <c r="C14" t="s">
         <v>26</v>
       </c>
-      <c r="D14" s="1"/>
-      <c r="E14" s="2">
+      <c r="E14" s="1">
         <v>43305</v>
       </c>
       <c r="F14" t="s">
@@ -1037,11 +1076,10 @@
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C15" s="1" t="s">
+      <c r="C15" t="s">
         <v>24</v>
       </c>
-      <c r="D15" s="1"/>
-      <c r="E15" s="2">
+      <c r="E15" s="1">
         <v>43306</v>
       </c>
       <c r="F15" t="s">
@@ -1052,11 +1090,10 @@
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C16" s="1" t="s">
+      <c r="C16" t="s">
         <v>25</v>
       </c>
-      <c r="D16" s="1"/>
-      <c r="E16" s="2">
+      <c r="E16" s="1">
         <v>43306</v>
       </c>
       <c r="F16" t="s">
@@ -1067,11 +1104,10 @@
       </c>
     </row>
     <row r="17" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C17" s="1" t="s">
+      <c r="C17" t="s">
         <v>23</v>
       </c>
-      <c r="D17" s="1"/>
-      <c r="E17" s="3">
+      <c r="E17" s="1">
         <v>43307</v>
       </c>
       <c r="F17" t="s">
@@ -1082,11 +1118,10 @@
       </c>
     </row>
     <row r="18" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C18" s="1" t="s">
+      <c r="C18" t="s">
         <v>22</v>
       </c>
-      <c r="D18" s="1"/>
-      <c r="E18" s="2">
+      <c r="E18" s="1">
         <v>43308</v>
       </c>
       <c r="F18" t="s">
@@ -1097,11 +1132,10 @@
       </c>
     </row>
     <row r="19" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C19" s="5" t="s">
+      <c r="C19" t="s">
         <v>39</v>
       </c>
-      <c r="D19" s="5"/>
-      <c r="E19" s="3">
+      <c r="E19" s="1">
         <v>43309</v>
       </c>
       <c r="F19" t="s">
@@ -1112,11 +1146,10 @@
       </c>
     </row>
     <row r="20" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C20" s="1" t="s">
+      <c r="C20" t="s">
         <v>20</v>
       </c>
-      <c r="D20" s="1"/>
-      <c r="E20" s="3">
+      <c r="E20" s="1">
         <v>43310</v>
       </c>
       <c r="F20" t="s">
@@ -1130,11 +1163,10 @@
       </c>
     </row>
     <row r="21" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C21" s="1" t="s">
+      <c r="C21" t="s">
         <v>21</v>
       </c>
-      <c r="D21" s="1"/>
-      <c r="E21" s="2">
+      <c r="E21" s="1">
         <v>43310</v>
       </c>
       <c r="F21" t="s">
@@ -1142,11 +1174,10 @@
       </c>
     </row>
     <row r="22" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C22" s="1" t="s">
+      <c r="C22" t="s">
         <v>17</v>
       </c>
-      <c r="D22" s="1"/>
-      <c r="E22" s="3">
+      <c r="E22" s="1">
         <v>43311</v>
       </c>
       <c r="F22" t="s">
@@ -1154,11 +1185,10 @@
       </c>
     </row>
     <row r="23" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C23" s="1" t="s">
+      <c r="C23" t="s">
         <v>18</v>
       </c>
-      <c r="D23" s="1"/>
-      <c r="E23" s="2">
+      <c r="E23" s="1">
         <v>43311</v>
       </c>
       <c r="F23" t="s">
@@ -1172,11 +1202,10 @@
       </c>
     </row>
     <row r="24" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C24" s="1" t="s">
+      <c r="C24" t="s">
         <v>19</v>
       </c>
-      <c r="D24" s="1"/>
-      <c r="E24" s="3">
+      <c r="E24" s="1">
         <v>43311</v>
       </c>
       <c r="F24" t="s">
@@ -1187,11 +1216,10 @@
       </c>
     </row>
     <row r="25" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C25" s="1" t="s">
+      <c r="C25" t="s">
         <v>16</v>
       </c>
-      <c r="D25" s="1"/>
-      <c r="E25" s="3">
+      <c r="E25" s="1">
         <v>43312</v>
       </c>
       <c r="F25" t="s">
@@ -1205,11 +1233,10 @@
       </c>
     </row>
     <row r="26" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C26" s="1" t="s">
+      <c r="C26" t="s">
         <v>15</v>
       </c>
-      <c r="D26" s="1"/>
-      <c r="E26" s="3">
+      <c r="E26" s="1">
         <v>43313</v>
       </c>
       <c r="F26" t="s">
@@ -1223,13 +1250,13 @@
       </c>
     </row>
     <row r="27" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C27" s="1" t="s">
+      <c r="C27" t="s">
         <v>13</v>
       </c>
-      <c r="D27" s="1">
+      <c r="D27">
         <v>2</v>
       </c>
-      <c r="E27" s="3">
+      <c r="E27" s="1">
         <v>43314</v>
       </c>
       <c r="F27" t="s">
@@ -1243,11 +1270,10 @@
       </c>
     </row>
     <row r="28" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C28" s="1" t="s">
+      <c r="C28" t="s">
         <v>14</v>
       </c>
-      <c r="D28" s="1"/>
-      <c r="E28" s="3">
+      <c r="E28" s="1">
         <v>43314</v>
       </c>
       <c r="F28" t="s">
@@ -1258,11 +1284,10 @@
       </c>
     </row>
     <row r="29" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C29" s="1" t="s">
+      <c r="C29" t="s">
         <v>54</v>
       </c>
-      <c r="D29" s="1"/>
-      <c r="E29" s="3">
+      <c r="E29" s="1">
         <v>43315</v>
       </c>
       <c r="F29" t="s">
@@ -1270,11 +1295,10 @@
       </c>
     </row>
     <row r="30" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C30" s="1" t="s">
+      <c r="C30" t="s">
         <v>55</v>
       </c>
-      <c r="D30" s="1"/>
-      <c r="E30" s="3">
+      <c r="E30" s="1">
         <v>43315</v>
       </c>
       <c r="F30" t="s">
@@ -1282,11 +1306,10 @@
       </c>
     </row>
     <row r="31" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C31" s="1" t="s">
+      <c r="C31" t="s">
         <v>12</v>
       </c>
-      <c r="D31" s="1"/>
-      <c r="E31" s="3">
+      <c r="E31" s="1">
         <v>43316</v>
       </c>
       <c r="F31" t="s">
@@ -1300,13 +1323,13 @@
       </c>
     </row>
     <row r="32" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C32" s="1" t="s">
+      <c r="C32" t="s">
         <v>12</v>
       </c>
-      <c r="D32" s="1">
+      <c r="D32">
         <v>2</v>
       </c>
-      <c r="E32" s="3">
+      <c r="E32" s="1">
         <v>43316</v>
       </c>
       <c r="F32" t="s">
@@ -1320,11 +1343,10 @@
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C33" s="5" t="s">
+      <c r="C33" t="s">
         <v>38</v>
       </c>
-      <c r="D33" s="5"/>
-      <c r="E33" s="3">
+      <c r="E33" s="1">
         <v>43316</v>
       </c>
       <c r="F33" t="s">
@@ -1332,11 +1354,10 @@
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C34" s="1" t="s">
+      <c r="C34" t="s">
         <v>11</v>
       </c>
-      <c r="D34" s="1"/>
-      <c r="E34" s="3">
+      <c r="E34" s="1">
         <v>43318</v>
       </c>
       <c r="F34" t="s">
@@ -1350,11 +1371,10 @@
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C35" s="1" t="s">
+      <c r="C35" t="s">
         <v>10</v>
       </c>
-      <c r="D35" s="1"/>
-      <c r="E35" s="3">
+      <c r="E35" s="1">
         <v>43319</v>
       </c>
       <c r="F35" t="s">
@@ -1368,11 +1388,10 @@
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C36" s="1" t="s">
+      <c r="C36" t="s">
         <v>9</v>
       </c>
-      <c r="D36" s="1"/>
-      <c r="E36" s="3">
+      <c r="E36" s="1">
         <v>43320</v>
       </c>
       <c r="F36" t="s">
@@ -1383,11 +1402,10 @@
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C37" s="1" t="s">
+      <c r="C37" t="s">
         <v>7</v>
       </c>
-      <c r="D37" s="1"/>
-      <c r="E37" s="3">
+      <c r="E37" s="1">
         <v>43321</v>
       </c>
       <c r="F37" t="s">
@@ -1398,11 +1416,10 @@
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C38" s="1" t="s">
+      <c r="C38" t="s">
         <v>8</v>
       </c>
-      <c r="D38" s="1"/>
-      <c r="E38" s="3">
+      <c r="E38" s="1">
         <v>43321</v>
       </c>
       <c r="F38" t="s">
@@ -1416,13 +1433,13 @@
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C39" s="1" t="s">
+      <c r="C39" t="s">
         <v>112</v>
       </c>
-      <c r="D39" s="1">
+      <c r="D39">
         <v>3</v>
       </c>
-      <c r="E39" s="3">
+      <c r="E39" s="1">
         <v>43322</v>
       </c>
       <c r="F39" t="s">
@@ -1436,11 +1453,10 @@
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C40" s="1" t="s">
+      <c r="C40" t="s">
         <v>6</v>
       </c>
-      <c r="D40" s="1"/>
-      <c r="E40" s="3">
+      <c r="E40" s="1">
         <v>43323</v>
       </c>
       <c r="F40" t="s">
@@ -1454,11 +1470,10 @@
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C41" s="1" t="s">
+      <c r="C41" t="s">
         <v>4</v>
       </c>
-      <c r="D41" s="1"/>
-      <c r="E41" s="3">
+      <c r="E41" s="1">
         <v>43325</v>
       </c>
       <c r="F41" t="s">
@@ -1472,11 +1487,10 @@
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C42" s="1" t="s">
+      <c r="C42" t="s">
         <v>5</v>
       </c>
-      <c r="D42" s="1"/>
-      <c r="E42" s="3">
+      <c r="E42" s="1">
         <v>43325</v>
       </c>
       <c r="F42" t="s">
@@ -1487,11 +1501,10 @@
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C43" s="1" t="s">
+      <c r="C43" t="s">
         <v>2</v>
       </c>
-      <c r="D43" s="1"/>
-      <c r="E43" s="3">
+      <c r="E43" s="1">
         <v>43326</v>
       </c>
       <c r="F43" t="s">
@@ -1508,11 +1521,10 @@
       <c r="B44" t="s">
         <v>95</v>
       </c>
-      <c r="C44" s="1" t="s">
+      <c r="C44" t="s">
         <v>3</v>
       </c>
-      <c r="D44" s="1"/>
-      <c r="E44" s="3">
+      <c r="E44" s="1">
         <v>43328</v>
       </c>
       <c r="F44" t="s">
@@ -1532,11 +1544,10 @@
       <c r="B45" t="s">
         <v>94</v>
       </c>
-      <c r="C45" s="1" t="s">
+      <c r="C45" t="s">
         <v>0</v>
       </c>
-      <c r="D45" s="1"/>
-      <c r="E45" s="3">
+      <c r="E45" s="1">
         <v>43328</v>
       </c>
       <c r="F45" t="s">
@@ -1556,11 +1567,10 @@
       <c r="B46" t="s">
         <v>94</v>
       </c>
-      <c r="C46" s="1" t="s">
+      <c r="C46" t="s">
         <v>1</v>
       </c>
-      <c r="D46" s="1"/>
-      <c r="E46" s="3">
+      <c r="E46" s="1">
         <v>43328</v>
       </c>
       <c r="F46" t="s">
@@ -1574,11 +1584,10 @@
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C47" s="1" t="s">
+      <c r="C47" t="s">
         <v>113</v>
       </c>
-      <c r="D47" s="1"/>
-      <c r="E47" s="3">
+      <c r="E47" s="1">
         <v>43332</v>
       </c>
       <c r="F47" t="s">
@@ -1589,10 +1598,395 @@
       <c r="C48" t="s">
         <v>36</v>
       </c>
-      <c r="E48" s="3">
+      <c r="E48" s="1">
         <v>43332</v>
       </c>
       <c r="F48" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="49" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C49" t="s">
+        <v>36</v>
+      </c>
+      <c r="E49" s="1">
+        <v>43347</v>
+      </c>
+      <c r="F49" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="50" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C50" t="s">
+        <v>124</v>
+      </c>
+      <c r="E50" s="1">
+        <v>43348</v>
+      </c>
+      <c r="F50" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="51" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C51" t="s">
+        <v>150</v>
+      </c>
+      <c r="E51" s="1">
+        <v>43349</v>
+      </c>
+      <c r="F51" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="52" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C52" t="s">
+        <v>125</v>
+      </c>
+      <c r="E52" s="1">
+        <v>43350</v>
+      </c>
+      <c r="F52" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="53" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C53" t="s">
+        <v>126</v>
+      </c>
+      <c r="E53" s="1">
+        <v>43351</v>
+      </c>
+      <c r="F53" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="54" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C54" t="s">
+        <v>127</v>
+      </c>
+      <c r="E54" s="1">
+        <v>43352</v>
+      </c>
+      <c r="F54" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="55" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C55" t="s">
+        <v>128</v>
+      </c>
+      <c r="E55" s="1">
+        <v>43353</v>
+      </c>
+      <c r="F55" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="56" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C56" t="s">
+        <v>129</v>
+      </c>
+      <c r="E56" s="1">
+        <v>43354</v>
+      </c>
+      <c r="F56" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="57" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C57" t="s">
+        <v>129</v>
+      </c>
+      <c r="E57" s="1">
+        <v>43355</v>
+      </c>
+      <c r="F57" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="58" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C58" t="s">
+        <v>130</v>
+      </c>
+      <c r="E58" s="1">
+        <v>43356</v>
+      </c>
+      <c r="F58" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="59" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C59" t="s">
+        <v>131</v>
+      </c>
+      <c r="E59" s="1">
+        <v>43357</v>
+      </c>
+      <c r="F59" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="60" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C60" t="s">
+        <v>132</v>
+      </c>
+      <c r="E60" s="1">
+        <v>43358</v>
+      </c>
+      <c r="F60" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="61" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C61" t="s">
+        <v>133</v>
+      </c>
+      <c r="E61" s="1">
+        <v>43359</v>
+      </c>
+      <c r="F61" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="62" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C62" t="s">
+        <v>134</v>
+      </c>
+      <c r="E62" s="1">
+        <v>43360</v>
+      </c>
+      <c r="F62" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="63" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C63" t="s">
+        <v>135</v>
+      </c>
+      <c r="E63" s="1">
+        <v>43361</v>
+      </c>
+      <c r="F63" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="64" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C64" t="s">
+        <v>136</v>
+      </c>
+      <c r="E64" s="1">
+        <v>43362</v>
+      </c>
+      <c r="F64" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="65" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C65" t="s">
+        <v>137</v>
+      </c>
+      <c r="E65" s="1">
+        <v>43363</v>
+      </c>
+      <c r="F65" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="66" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C66" t="s">
+        <v>137</v>
+      </c>
+      <c r="E66" s="1">
+        <v>43364</v>
+      </c>
+      <c r="F66" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="67" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C67" t="s">
+        <v>138</v>
+      </c>
+      <c r="E67" s="1">
+        <v>43365</v>
+      </c>
+      <c r="F67" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="68" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C68" t="s">
+        <v>139</v>
+      </c>
+      <c r="E68" s="1">
+        <v>43366</v>
+      </c>
+      <c r="F68" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="69" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C69" t="s">
+        <v>140</v>
+      </c>
+      <c r="E69" s="1">
+        <v>43367</v>
+      </c>
+      <c r="F69" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="70" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C70" t="s">
+        <v>140</v>
+      </c>
+      <c r="E70" s="1">
+        <v>43368</v>
+      </c>
+      <c r="F70" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="71" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C71" t="s">
+        <v>139</v>
+      </c>
+      <c r="E71" s="1">
+        <v>43369</v>
+      </c>
+      <c r="F71" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="72" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C72" t="s">
+        <v>138</v>
+      </c>
+      <c r="E72" s="1">
+        <v>43370</v>
+      </c>
+      <c r="F72" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="73" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C73" t="s">
+        <v>141</v>
+      </c>
+      <c r="E73" s="1">
+        <v>43371</v>
+      </c>
+      <c r="F73" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="74" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C74" t="s">
+        <v>142</v>
+      </c>
+      <c r="E74" s="1">
+        <v>43372</v>
+      </c>
+      <c r="F74" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="75" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C75" t="s">
+        <v>143</v>
+      </c>
+      <c r="E75" s="1">
+        <v>43373</v>
+      </c>
+      <c r="F75" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="76" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C76" t="s">
+        <v>144</v>
+      </c>
+      <c r="E76" s="1">
+        <v>43374</v>
+      </c>
+      <c r="F76" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="77" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C77" t="s">
+        <v>145</v>
+      </c>
+      <c r="E77" s="1">
+        <v>43375</v>
+      </c>
+      <c r="F77" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="78" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C78" t="s">
+        <v>146</v>
+      </c>
+      <c r="E78" s="1">
+        <v>43376</v>
+      </c>
+      <c r="F78" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="79" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C79" t="s">
+        <v>147</v>
+      </c>
+      <c r="E79" s="1">
+        <v>43377</v>
+      </c>
+      <c r="F79" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="80" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C80" t="s">
+        <v>148</v>
+      </c>
+      <c r="E80" s="1">
+        <v>43378</v>
+      </c>
+      <c r="F80" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="81" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C81" t="s">
+        <v>148</v>
+      </c>
+      <c r="E81" s="1">
+        <v>43379</v>
+      </c>
+      <c r="F81" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="82" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C82" t="s">
+        <v>149</v>
+      </c>
+      <c r="E82" s="1">
+        <v>43380</v>
+      </c>
+      <c r="F82" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="83" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C83" t="s">
+        <v>36</v>
+      </c>
+      <c r="E83" s="1">
+        <v>43383</v>
+      </c>
+      <c r="F83" t="s">
         <v>37</v>
       </c>
     </row>

</xml_diff>